<commit_message>
Correctly assign chat messages to employees and improve data integrity
Fixes incorrect employee assignments in chat_messages table, enhancing data accuracy.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 1c1ae5fa-441a-4286-8ccf-43a6b2d438fb
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/44d5a101-b4ed-4c60-a589-dbb63326a349/e02f5952-a3a9-4025-a4b7-bcc05d432434.jpg
</commit_message>
<xml_diff>
--- a/Chat_Messages_Export_2025-07-06.xlsx
+++ b/Chat_Messages_Export_2025-07-06.xlsx
@@ -490,7 +490,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>316</v>
+        <v>365</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -514,18 +514,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I3" t="str">
-        <v xml:space="preserve">There is no active opportunity at the moment. Mahaveer intends to provide him  in Optimizely </v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J3" t="str">
-        <v>6/25/2025, 7:42:31 PM</v>
+        <v>6/25/2025, 7:43:19 PM</v>
       </c>
       <c r="K3">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -549,18 +549,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I4" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case - Wild fork use case</v>
       </c>
       <c r="J4" t="str">
-        <v>6/25/2025, 7:43:19 PM</v>
+        <v>6/25/2025, 7:44:15 PM</v>
       </c>
       <c r="K4">
-        <v>109</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -584,18 +584,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I5" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case - Wild fork use case</v>
+        <v>Managing - PlaceMaker &amp; Pet Barn ( AREN) - Cost covered in the Margin</v>
       </c>
       <c r="J5" t="str">
-        <v>6/25/2025, 7:44:15 PM</v>
+        <v>6/25/2025, 7:56:10 PM</v>
       </c>
       <c r="K5">
-        <v>130</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -619,18 +619,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I6" t="str">
-        <v>Managing - PlaceMaker &amp; Pet Barn ( AREN) - Cost covered in the Margin</v>
+        <v>Managing MENA Bev and JBS accounts, acting as an account manager for the Pakistan-based operations—currently covered under MENA Bev.</v>
       </c>
       <c r="J6" t="str">
-        <v>6/25/2025, 7:56:10 PM</v>
+        <v>6/25/2025, 7:58:06 PM</v>
       </c>
       <c r="K6">
-        <v>69</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>338</v>
+        <v>266</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -654,18 +654,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I7" t="str">
-        <v>Managing MENA Bev and JBS accounts, acting as an account manager for the Pakistan-based operations—currently covered under MENA Bev.</v>
+        <v xml:space="preserve">PM for Y design &amp; True religion, From Aug Bellacor - 50 % billable - SOW is under preparation </v>
       </c>
       <c r="J7" t="str">
-        <v>6/25/2025, 7:58:06 PM</v>
+        <v>6/25/2025, 8:02:51 PM</v>
       </c>
       <c r="K7">
-        <v>132</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>266</v>
+        <v>329</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -689,18 +689,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I8" t="str">
-        <v xml:space="preserve">PM for Y design &amp; True religion, From Aug Bellacor - 50 % billable - SOW is under preparation </v>
+        <v>He is currently working in maintenance and will become billable starting from July 3rd</v>
       </c>
       <c r="J8" t="str">
-        <v>6/25/2025, 8:02:51 PM</v>
+        <v>6/25/2025, 8:03:58 PM</v>
       </c>
       <c r="K8">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>329</v>
+        <v>375</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -724,18 +724,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I9" t="str">
-        <v>He is currently working in maintenance and will become billable starting from July 3rd</v>
+        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
       </c>
       <c r="J9" t="str">
-        <v>6/25/2025, 8:03:58 PM</v>
+        <v>6/25/2025, 8:06:23 PM</v>
       </c>
       <c r="K9">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>375</v>
+        <v>307</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -759,18 +759,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I10" t="str">
-        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
+        <v>One and only React bench resource. (Plan for Training)</v>
       </c>
       <c r="J10" t="str">
-        <v>6/25/2025, 8:06:23 PM</v>
+        <v>6/25/2025, 8:07:57 PM</v>
       </c>
       <c r="K10">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -794,18 +794,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I11" t="str">
-        <v>One and only React bench resource. (Plan for Training)</v>
+        <v>Was billable in Dimond Roofing - Fletcher Builder. Moved to bench from 23rd June</v>
       </c>
       <c r="J11" t="str">
-        <v>6/25/2025, 8:07:57 PM</v>
+        <v>6/27/2025, 5:24:09 PM</v>
       </c>
       <c r="K11">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -829,18 +829,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I12" t="str">
-        <v>Was billable in Dimond Roofing - Fletcher Builder. Moved to bench from 23rd June</v>
+        <v>50% Billable in Whilecap . Aslo PM for - Rockwest, UFA</v>
       </c>
       <c r="J12" t="str">
-        <v>6/27/2025, 5:24:09 PM</v>
+        <v>7/2/2025, 8:17:19 PM</v>
       </c>
       <c r="K12">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -864,18 +864,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I13" t="str">
-        <v>50% Billable in Whilecap . Aslo PM for - Rockwest, UFA</v>
+        <v xml:space="preserve">No billable SOW - 7 Billable and 1 Non Billable to cover -  24X 7 Project &amp; Back Up </v>
       </c>
       <c r="J13" t="str">
-        <v>7/2/2025, 8:17:19 PM</v>
+        <v>7/2/2025, 8:28:30 PM</v>
       </c>
       <c r="K13">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>260</v>
+        <v>359</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -896,21 +896,21 @@
         <v>AI Training</v>
       </c>
       <c r="H14" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Karthik Venkittu</v>
       </c>
       <c r="I14" t="str">
-        <v xml:space="preserve">No billable SOW - 7 Billable and 1 Non Billable to cover -  24X 7 Project &amp; Back Up </v>
+        <v>He is working for Client HD Supply. Non-billable shadow resource for the 24*7 support. He is part of the signed SOW.</v>
       </c>
       <c r="J14" t="str">
-        <v>7/2/2025, 8:28:30 PM</v>
+        <v>7/3/2025, 12:31:52 PM</v>
       </c>
       <c r="K14">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>359</v>
+        <v>300</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -934,18 +934,18 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I15" t="str">
-        <v>He is working for Client HD Supply. Non-billable shadow resource for the 24*7 support. He is part of the signed SOW.</v>
+        <v>Offboarded on 30th June</v>
       </c>
       <c r="J15" t="str">
-        <v>7/3/2025, 12:31:52 PM</v>
+        <v>7/3/2025, 12:43:05 PM</v>
       </c>
       <c r="K15">
-        <v>116</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>300</v>
+        <v>382</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -966,30 +966,30 @@
         <v>AI Training</v>
       </c>
       <c r="H16" t="str">
-        <v>Karthik Venkittu</v>
+        <v>Muhammad Rehman Shahid</v>
       </c>
       <c r="I16" t="str">
-        <v>Offboarded on 30th June</v>
+        <v>This is test comments by Rehman on 6th July at 10:07 AM PK Time</v>
       </c>
       <c r="J16" t="str">
-        <v>7/3/2025, 12:43:05 PM</v>
+        <v>7/6/2025, 5:08:01 AM</v>
       </c>
       <c r="K16">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>382</v>
+        <v>298</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="str">
-        <v>10000011</v>
+        <v>10000091</v>
       </c>
       <c r="D17" t="str">
-        <v>M Abdullah Ansari</v>
+        <v>Kishor Kumar Sahu</v>
       </c>
       <c r="E17" t="str">
         <v>AI Innovation</v>
@@ -1001,21 +1001,21 @@
         <v>AI Training</v>
       </c>
       <c r="H17" t="str">
-        <v>Muhammad Rehman Shahid</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I17" t="str">
-        <v>This is test comments by Rehman on 6th July at 10:07 AM PK Time</v>
+        <v xml:space="preserve">Practice .. just release from MARS... </v>
       </c>
       <c r="J17" t="str">
-        <v>7/6/2025, 5:08:01 AM</v>
+        <v>6/23/2025, 6:49:38 PM</v>
       </c>
       <c r="K17">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1036,21 +1036,21 @@
         <v>AI Training</v>
       </c>
       <c r="H18" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I18" t="str">
-        <v xml:space="preserve">Practice .. just release from MARS... </v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training</v>
       </c>
       <c r="J18" t="str">
-        <v>6/23/2025, 6:49:38 PM</v>
+        <v>6/25/2025, 7:41:43 PM</v>
       </c>
       <c r="K18">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>363</v>
+        <v>262</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1074,13 +1074,13 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I19" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training</v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J19" t="str">
-        <v>6/25/2025, 7:41:43 PM</v>
+        <v>6/25/2025, 7:45:04 PM</v>
       </c>
       <c r="K19">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1144,18 +1144,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I21" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
+        <v>50% Billable in Whilecap . Also PM for - Rockwest, UFA</v>
       </c>
       <c r="J21" t="str">
-        <v>6/25/2025, 7:45:04 PM</v>
+        <v>6/25/2025, 7:52:38 PM</v>
       </c>
       <c r="K21">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>291</v>
+        <v>349</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1179,18 +1179,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I22" t="str">
-        <v>50% Billable in Whilecap . Also PM for - Rockwest, UFA</v>
+        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
       </c>
       <c r="J22" t="str">
-        <v>6/25/2025, 7:52:38 PM</v>
+        <v>6/25/2025, 7:58:34 PM</v>
       </c>
       <c r="K22">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>349</v>
+        <v>267</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1214,18 +1214,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I23" t="str">
-        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
+        <v xml:space="preserve">PM for Y design &amp; True religion, From Aug Bellacor - 50 % billable - SOW is under preparation </v>
       </c>
       <c r="J23" t="str">
-        <v>6/25/2025, 7:58:34 PM</v>
+        <v>6/25/2025, 8:02:51 PM</v>
       </c>
       <c r="K23">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1249,18 +1249,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I24" t="str">
-        <v xml:space="preserve">PM for Y design &amp; True religion, From Aug Bellacor - 50 % billable - SOW is under preparation </v>
+        <v>One and only React bench resource. (Plan for Training)</v>
       </c>
       <c r="J24" t="str">
-        <v>6/25/2025, 8:02:51 PM</v>
+        <v>6/25/2025, 8:07:56 PM</v>
       </c>
       <c r="K24">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1281,21 +1281,21 @@
         <v>AI Training</v>
       </c>
       <c r="H25" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Muhammad Rehman Shahid</v>
       </c>
       <c r="I25" t="str">
-        <v>One and only React bench resource. (Plan for Training)</v>
+        <v>This is 3rd test comments added by Rehman</v>
       </c>
       <c r="J25" t="str">
-        <v>6/25/2025, 8:07:56 PM</v>
+        <v>6/26/2025, 3:38:40 PM</v>
       </c>
       <c r="K25">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1316,21 +1316,21 @@
         <v>AI Training</v>
       </c>
       <c r="H26" t="str">
-        <v>Muhammad Rehman Shahid</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I26" t="str">
-        <v>This is 3rd test comments added by Rehman</v>
+        <v xml:space="preserve">He is working in maintance - From 3rd July he will be billable </v>
       </c>
       <c r="J26" t="str">
-        <v>6/26/2025, 3:38:40 PM</v>
+        <v>7/2/2025, 8:27:11 PM</v>
       </c>
       <c r="K26">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>331</v>
+        <v>284</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1354,18 +1354,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I27" t="str">
-        <v xml:space="preserve">He is working in maintance - From 3rd July he will be billable </v>
+        <v>Will be released from RAC by End of June. Nandha &amp;. Rama  will come back to us on or before 4th July</v>
       </c>
       <c r="J27" t="str">
-        <v>7/2/2025, 8:27:11 PM</v>
+        <v>7/2/2025, 8:41:25 PM</v>
       </c>
       <c r="K27">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1386,21 +1386,21 @@
         <v>AI Training</v>
       </c>
       <c r="H28" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Karthik Venkittu</v>
       </c>
       <c r="I28" t="str">
-        <v>Will be released from RAC by End of June. Nandha &amp;. Rama  will come back to us on or before 4th July</v>
+        <v>Resigned and LWD is 3rd July</v>
       </c>
       <c r="J28" t="str">
-        <v>7/2/2025, 8:41:25 PM</v>
+        <v>7/3/2025, 12:36:18 PM</v>
       </c>
       <c r="K28">
-        <v>100</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>275</v>
+        <v>323</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1421,21 +1421,21 @@
         <v>AI Training</v>
       </c>
       <c r="H29" t="str">
-        <v>Karthik Venkittu</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I29" t="str">
-        <v>Resigned and LWD is 3rd July</v>
+        <v>Managing - Barns and Noble, CEGB, JSW -  Will be billable 100% in MOS from JULY</v>
       </c>
       <c r="J29" t="str">
-        <v>7/3/2025, 12:36:18 PM</v>
+        <v>7/3/2025, 1:24:52 PM</v>
       </c>
       <c r="K29">
-        <v>28</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>323</v>
+        <v>378</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1459,18 +1459,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I30" t="str">
-        <v>Managing - Barns and Noble, CEGB, JSW -  Will be billable 100% in MOS from JULY</v>
+        <v>Managing - Mena bev, JBS - Like a account manager for Pakistan base- Covered under Mena bev</v>
       </c>
       <c r="J30" t="str">
-        <v>7/3/2025, 1:24:52 PM</v>
+        <v>7/3/2025, 1:25:26 PM</v>
       </c>
       <c r="K30">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>378</v>
+        <v>341</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1494,18 +1494,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I31" t="str">
-        <v>Managing - Mena bev, JBS - Like a account manager for Pakistan base- Covered under Mena bev</v>
+        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
       </c>
       <c r="J31" t="str">
-        <v>7/3/2025, 1:25:26 PM</v>
+        <v>7/3/2025, 1:26:09 PM</v>
       </c>
       <c r="K31">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1529,10 +1529,10 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I32" t="str">
-        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
+        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
       </c>
       <c r="J32" t="str">
-        <v>7/3/2025, 1:26:09 PM</v>
+        <v>7/3/2025, 1:26:37 PM</v>
       </c>
       <c r="K32">
         <v>75</v>
@@ -1540,16 +1540,16 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>362</v>
+        <v>299</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="str">
-        <v>10000091</v>
+        <v>10000211</v>
       </c>
       <c r="D33" t="str">
-        <v>Kishor Kumar Sahu</v>
+        <v>Karthik  Kanaparthi</v>
       </c>
       <c r="E33" t="str">
         <v>AI Innovation</v>
@@ -1561,21 +1561,21 @@
         <v>AI Training</v>
       </c>
       <c r="H33" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I33" t="str">
-        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
+        <v xml:space="preserve">Practice .. just release from MARS... </v>
       </c>
       <c r="J33" t="str">
-        <v>7/3/2025, 1:26:37 PM</v>
+        <v>6/23/2025, 6:49:38 PM</v>
       </c>
       <c r="K33">
-        <v>75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1596,21 +1596,21 @@
         <v>AI Training</v>
       </c>
       <c r="H34" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I34" t="str">
-        <v xml:space="preserve">Practice .. just release from MARS... </v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training</v>
       </c>
       <c r="J34" t="str">
-        <v>6/23/2025, 6:49:38 PM</v>
+        <v>6/25/2025, 7:41:43 PM</v>
       </c>
       <c r="K34">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>364</v>
+        <v>292</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -1634,18 +1634,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I35" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training</v>
+        <v>50% Billable in Whilecap . Also PM for - Rockwest, UFA</v>
       </c>
       <c r="J35" t="str">
-        <v>6/25/2025, 7:41:43 PM</v>
+        <v>6/25/2025, 7:52:38 PM</v>
       </c>
       <c r="K35">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>292</v>
+        <v>350</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -1669,18 +1669,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I36" t="str">
-        <v>50% Billable in Whilecap . Also PM for - Rockwest, UFA</v>
+        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
       </c>
       <c r="J36" t="str">
-        <v>6/25/2025, 7:52:38 PM</v>
+        <v>6/25/2025, 7:58:34 PM</v>
       </c>
       <c r="K36">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -1704,10 +1704,10 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I37" t="str">
-        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
+        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
       </c>
       <c r="J37" t="str">
-        <v>6/25/2025, 7:58:34 PM</v>
+        <v>6/25/2025, 8:01:28 PM</v>
       </c>
       <c r="K37">
         <v>75</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -1739,18 +1739,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I38" t="str">
-        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
+        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
       </c>
       <c r="J38" t="str">
-        <v>6/25/2025, 8:01:28 PM</v>
+        <v>6/25/2025, 8:08:16 PM</v>
       </c>
       <c r="K38">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -1771,21 +1771,21 @@
         <v>AI Training</v>
       </c>
       <c r="H39" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Muhammad Rehman Shahid</v>
       </c>
       <c r="I39" t="str">
-        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
+        <v>This is 3rd test comments added by Rehman</v>
       </c>
       <c r="J39" t="str">
-        <v>6/25/2025, 8:08:16 PM</v>
+        <v>6/26/2025, 3:38:39 PM</v>
       </c>
       <c r="K39">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>321</v>
+        <v>268</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1806,21 +1806,21 @@
         <v>AI Training</v>
       </c>
       <c r="H40" t="str">
-        <v>Muhammad Rehman Shahid</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I40" t="str">
-        <v>This is 3rd test comments added by Rehman</v>
+        <v>Was on leave entire last week</v>
       </c>
       <c r="J40" t="str">
-        <v>6/26/2025, 3:38:39 PM</v>
+        <v>6/27/2025, 5:17:32 PM</v>
       </c>
       <c r="K40">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -1844,18 +1844,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I41" t="str">
-        <v>Was on leave entire last week</v>
+        <v>T&amp;M work starting in Dimond+/Laminex NZ project starting from July 14th for 2 months</v>
       </c>
       <c r="J41" t="str">
-        <v>6/27/2025, 5:17:32 PM</v>
+        <v>6/30/2025, 5:55:18 PM</v>
       </c>
       <c r="K41">
-        <v>29</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>283</v>
+        <v>340</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1879,18 +1879,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I42" t="str">
-        <v>T&amp;M work starting in Dimond+/Laminex NZ project starting from July 14th for 2 months</v>
+        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
       </c>
       <c r="J42" t="str">
-        <v>6/30/2025, 5:55:18 PM</v>
+        <v>7/2/2025, 8:23:53 PM</v>
       </c>
       <c r="K42">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>340</v>
+        <v>377</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1911,21 +1911,21 @@
         <v>AI Training</v>
       </c>
       <c r="H43" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Karthik Venkittu</v>
       </c>
       <c r="I43" t="str">
-        <v xml:space="preserve">Managing - Arcelik, Dollance , Arceli Hitachi - Cost Covered in the Margin </v>
+        <v>Moved to RAC project effective from 1st July</v>
       </c>
       <c r="J43" t="str">
-        <v>7/2/2025, 8:23:53 PM</v>
+        <v>7/3/2025, 12:38:22 PM</v>
       </c>
       <c r="K43">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>377</v>
+        <v>332</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -1949,18 +1949,18 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I44" t="str">
-        <v>Moved to RAC project effective from 1st July</v>
+        <v>Moved to Agriserv project effective from 3rd July</v>
       </c>
       <c r="J44" t="str">
-        <v>7/3/2025, 12:38:22 PM</v>
+        <v>7/3/2025, 12:39:31 PM</v>
       </c>
       <c r="K44">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>332</v>
+        <v>279</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -1984,18 +1984,18 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I45" t="str">
-        <v>Moved to Agriserv project effective from 3rd July</v>
+        <v xml:space="preserve">She will be made billable from 1st August in RAC SFB2CComposable Migration project. SOW is in the process. </v>
       </c>
       <c r="J45" t="str">
-        <v>7/3/2025, 12:39:31 PM</v>
+        <v>7/3/2025, 12:56:44 PM</v>
       </c>
       <c r="K45">
-        <v>49</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2019,27 +2019,27 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I46" t="str">
-        <v xml:space="preserve">She will be made billable from 1st August in RAC SFB2CComposable Migration project. SOW is in the process. </v>
+        <v>Working on AI solutions and will be mapped in MARS during 1st week of September</v>
       </c>
       <c r="J46" t="str">
-        <v>7/3/2025, 12:56:44 PM</v>
+        <v>7/3/2025, 1:04:13 PM</v>
       </c>
       <c r="K46">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>308</v>
+        <v>347</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" t="str">
-        <v>10000211</v>
+        <v>10000261</v>
       </c>
       <c r="D47" t="str">
-        <v>Karthik  Kanaparthi</v>
+        <v>Kishore Babu Meduri</v>
       </c>
       <c r="E47" t="str">
         <v>AI Innovation</v>
@@ -2051,21 +2051,21 @@
         <v>AI Training</v>
       </c>
       <c r="H47" t="str">
-        <v>Karthik Venkittu</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I47" t="str">
-        <v>Working on AI solutions and will be mapped in MARS during 1st week of September</v>
+        <v>Released from Wildfork and can't find any billable oppurnitiny. So, releasing from the org. &gt;tried one month for AI training but she cant able to pickup.</v>
       </c>
       <c r="J47" t="str">
-        <v>7/3/2025, 1:04:13 PM</v>
+        <v>6/23/2025, 6:53:03 PM</v>
       </c>
       <c r="K47">
-        <v>79</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -2086,21 +2086,21 @@
         <v>AI Training</v>
       </c>
       <c r="H48" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I48" t="str">
-        <v>Released from Wildfork and can't find any billable oppurnitiny. So, releasing from the org. &gt;tried one month for AI training but she cant able to pickup.</v>
+        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
       </c>
       <c r="J48" t="str">
-        <v>6/23/2025, 6:53:03 PM</v>
+        <v>6/25/2025, 8:01:27 PM</v>
       </c>
       <c r="K48">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>360</v>
+        <v>263</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -2124,18 +2124,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I49" t="str">
-        <v xml:space="preserve">25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
+        <v xml:space="preserve">No billable SOW - 7 Billable and 1 Non Billable to cover -  24X 7 Project &amp; Back Up </v>
       </c>
       <c r="J49" t="str">
-        <v>6/25/2025, 8:01:27 PM</v>
+        <v>6/25/2025, 8:07:00 PM</v>
       </c>
       <c r="K49">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>264</v>
+        <v>325</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -2194,18 +2194,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I51" t="str">
-        <v xml:space="preserve">No billable SOW - 7 Billable and 1 Non Billable to cover -  24X 7 Project &amp; Back Up </v>
+        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
       </c>
       <c r="J51" t="str">
-        <v>6/25/2025, 8:07:00 PM</v>
+        <v>6/25/2025, 8:08:16 PM</v>
       </c>
       <c r="K51">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -2229,18 +2229,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I52" t="str">
-        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
+        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
       </c>
       <c r="J52" t="str">
-        <v>6/25/2025, 8:08:16 PM</v>
+        <v>6/25/2025, 8:08:38 PM</v>
       </c>
       <c r="K52">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>333</v>
+        <v>370</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -2264,18 +2264,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I53" t="str">
-        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
+        <v>RAC - ACIMA Extended Aisle - Bench from 1st June</v>
       </c>
       <c r="J53" t="str">
-        <v>6/25/2025, 8:08:38 PM</v>
+        <v>6/25/2025, 8:09:21 PM</v>
       </c>
       <c r="K53">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>370</v>
+        <v>285</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -2299,18 +2299,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I54" t="str">
-        <v>RAC - ACIMA Extended Aisle - Bench from 1st June</v>
+        <v>Will be released from RAC by End of June.</v>
       </c>
       <c r="J54" t="str">
-        <v>6/25/2025, 8:09:21 PM</v>
+        <v>6/25/2025, 8:10:45 PM</v>
       </c>
       <c r="K54">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -2331,21 +2331,21 @@
         <v>AI Training</v>
       </c>
       <c r="H55" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Farhan Ahmed</v>
       </c>
       <c r="I55" t="str">
-        <v>Will be released from RAC by End of June.</v>
+        <v>Test comment 2</v>
       </c>
       <c r="J55" t="str">
-        <v>6/25/2025, 8:10:45 PM</v>
+        <v>6/26/2025, 3:37:06 PM</v>
       </c>
       <c r="K55">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -2369,18 +2369,18 @@
         <v>Farhan Ahmed</v>
       </c>
       <c r="I56" t="str">
-        <v>Test comment 2</v>
+        <v>He is a Non-Billable PM at Richardson Sport</v>
       </c>
       <c r="J56" t="str">
-        <v>6/26/2025, 3:37:06 PM</v>
+        <v>6/26/2025, 3:45:03 PM</v>
       </c>
       <c r="K56">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -2401,21 +2401,21 @@
         <v>AI Training</v>
       </c>
       <c r="H57" t="str">
-        <v>Farhan Ahmed</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I57" t="str">
-        <v>He is a Non-Billable PM at Richardson Sport</v>
+        <v>under the FMLA to take up to 26 weeks of unpaid, job-protected FMLA leave in a single 12-month period</v>
       </c>
       <c r="J57" t="str">
-        <v>6/26/2025, 3:45:03 PM</v>
+        <v>6/27/2025, 5:21:45 PM</v>
       </c>
       <c r="K57">
-        <v>43</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2439,18 +2439,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I58" t="str">
-        <v>under the FMLA to take up to 26 weeks of unpaid, job-protected FMLA leave in a single 12-month period</v>
+        <v xml:space="preserve">Last working day - 30th June. </v>
       </c>
       <c r="J58" t="str">
-        <v>6/27/2025, 5:21:45 PM</v>
+        <v>6/30/2025, 5:07:20 PM</v>
       </c>
       <c r="K58">
-        <v>101</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -2477,7 +2477,7 @@
         <v xml:space="preserve">Last working day - 30th June. </v>
       </c>
       <c r="J59" t="str">
-        <v>6/30/2025, 5:07:20 PM</v>
+        <v>6/30/2025, 5:07:34 PM</v>
       </c>
       <c r="K59">
         <v>30</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>293</v>
+        <v>339</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -2512,7 +2512,7 @@
         <v xml:space="preserve">Last working day - 30th June. </v>
       </c>
       <c r="J60" t="str">
-        <v>6/30/2025, 5:07:34 PM</v>
+        <v>6/30/2025, 5:07:52 PM</v>
       </c>
       <c r="K60">
         <v>30</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>339</v>
+        <v>376</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -2544,18 +2544,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I61" t="str">
-        <v xml:space="preserve">Last working day - 30th June. </v>
+        <v>Managing - Mena bev, JBS - Like a account manager for Pakistan base- Covered under Mena bev</v>
       </c>
       <c r="J61" t="str">
-        <v>6/30/2025, 5:07:52 PM</v>
+        <v>7/2/2025, 8:23:32 PM</v>
       </c>
       <c r="K61">
-        <v>30</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>376</v>
+        <v>265</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -2579,18 +2579,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I62" t="str">
-        <v>Managing - Mena bev, JBS - Like a account manager for Pakistan base- Covered under Mena bev</v>
+        <v xml:space="preserve">Ignore the above comment - 25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
       </c>
       <c r="J62" t="str">
-        <v>7/2/2025, 8:23:32 PM</v>
+        <v>7/2/2025, 8:25:06 PM</v>
       </c>
       <c r="K62">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -2614,27 +2614,27 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I63" t="str">
-        <v xml:space="preserve">Ignore the above comment - 25% Billable in Augusta, From July we are expecting it to conver up to 50% </v>
+        <v>Off boarded - 30-Jun-2025</v>
       </c>
       <c r="J63" t="str">
-        <v>7/2/2025, 8:25:06 PM</v>
+        <v>7/2/2025, 8:51:20 PM</v>
       </c>
       <c r="K63">
-        <v>102</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" t="str">
-        <v>10000261</v>
+        <v>10000271</v>
       </c>
       <c r="D64" t="str">
-        <v>Kishore Babu Meduri</v>
+        <v>Kishore Chittabathina</v>
       </c>
       <c r="E64" t="str">
         <v>AI Innovation</v>
@@ -2646,21 +2646,21 @@
         <v>AI Training</v>
       </c>
       <c r="H64" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I64" t="str">
-        <v>Off boarded - 30-Jun-2025</v>
+        <v>Released from Wildfork and can't find any billable oppurnitiny. So, releasing from the org. &gt;tried one month for AI training but she cant able to pickup.</v>
       </c>
       <c r="J64" t="str">
-        <v>7/2/2025, 8:51:20 PM</v>
+        <v>6/23/2025, 6:53:03 PM</v>
       </c>
       <c r="K64">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -2681,21 +2681,21 @@
         <v>AI Training</v>
       </c>
       <c r="H65" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I65" t="str">
-        <v>Released from Wildfork and can't find any billable oppurnitiny. So, releasing from the org. &gt;tried one month for AI training but she cant able to pickup.</v>
+        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
       </c>
       <c r="J65" t="str">
-        <v>6/23/2025, 6:53:03 PM</v>
+        <v>6/25/2025, 8:08:38 PM</v>
       </c>
       <c r="K65">
-        <v>153</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -2719,18 +2719,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I66" t="str">
-        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
+        <v>RAC - ACIMA Extended Aisle - Bench from 1st June</v>
       </c>
       <c r="J66" t="str">
-        <v>6/25/2025, 8:08:38 PM</v>
+        <v>6/25/2025, 8:09:21 PM</v>
       </c>
       <c r="K66">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>371</v>
+        <v>286</v>
       </c>
       <c r="B67">
         <v>5</v>
@@ -2754,18 +2754,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I67" t="str">
-        <v>RAC - ACIMA Extended Aisle - Bench from 1st June</v>
+        <v>Will be released from RAC by End of June.</v>
       </c>
       <c r="J67" t="str">
-        <v>6/25/2025, 8:09:21 PM</v>
+        <v>6/25/2025, 8:10:45 PM</v>
       </c>
       <c r="K67">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>286</v>
+        <v>319</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -2786,21 +2786,21 @@
         <v>AI Training</v>
       </c>
       <c r="H68" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Farhan Ahmed</v>
       </c>
       <c r="I68" t="str">
-        <v>Will be released from RAC by End of June.</v>
+        <v>Test comment 2</v>
       </c>
       <c r="J68" t="str">
-        <v>6/25/2025, 8:10:45 PM</v>
+        <v>6/26/2025, 3:37:05 PM</v>
       </c>
       <c r="K68">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -2824,18 +2824,18 @@
         <v>Farhan Ahmed</v>
       </c>
       <c r="I69" t="str">
-        <v>Test comment 2</v>
+        <v>He is a Non-Billable PM at Richardson Sport</v>
       </c>
       <c r="J69" t="str">
-        <v>6/26/2025, 3:37:05 PM</v>
+        <v>6/26/2025, 3:45:02 PM</v>
       </c>
       <c r="K69">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" xml:space="preserve">
       <c r="A70">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -2856,21 +2856,22 @@
         <v>AI Training</v>
       </c>
       <c r="H70" t="str">
-        <v>Farhan Ahmed</v>
-      </c>
-      <c r="I70" t="str">
-        <v>He is a Non-Billable PM at Richardson Sport</v>
+        <v>Muhammad Rehman Shahid</v>
+      </c>
+      <c r="I70" t="str" xml:space="preserve">
+        <v xml:space="preserve">Abdullah is Non Billable._x000d_
+</v>
       </c>
       <c r="J70" t="str">
-        <v>6/26/2025, 3:45:02 PM</v>
+        <v>6/26/2025, 5:31:48 PM</v>
       </c>
       <c r="K70">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" xml:space="preserve">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71">
       <c r="A71">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -2891,22 +2892,21 @@
         <v>AI Training</v>
       </c>
       <c r="H71" t="str">
-        <v>Muhammad Rehman Shahid</v>
-      </c>
-      <c r="I71" t="str" xml:space="preserve">
-        <v xml:space="preserve">Abdullah is Non Billable._x000d_
-</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
+      </c>
+      <c r="I71" t="str">
+        <v>One and only React bench resource. (Plan for Training)</v>
       </c>
       <c r="J71" t="str">
-        <v>6/26/2025, 5:31:48 PM</v>
+        <v>6/30/2025, 5:54:43 PM</v>
       </c>
       <c r="K71">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B72">
         <v>5</v>
@@ -2930,18 +2930,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I72" t="str">
-        <v>One and only React bench resource. (Plan for Training)</v>
+        <v>Managing - Work Wear, Gallagher, Pet Barn</v>
       </c>
       <c r="J72" t="str">
-        <v>6/30/2025, 5:54:43 PM</v>
+        <v>7/2/2025, 8:17:44 PM</v>
       </c>
       <c r="K72">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -2965,18 +2965,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I73" t="str">
-        <v>Managing - Work Wear, Gallagher, Pet Barn</v>
+        <v xml:space="preserve">one and only React bench resource. Will Train the internal team in React </v>
       </c>
       <c r="J73" t="str">
-        <v>7/2/2025, 8:17:44 PM</v>
+        <v>7/2/2025, 8:39:11 PM</v>
       </c>
       <c r="K73">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="B74">
         <v>5</v>
@@ -3000,18 +3000,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I74" t="str">
-        <v xml:space="preserve">one and only React bench resource. Will Train the internal team in React </v>
+        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
       </c>
       <c r="J74" t="str">
-        <v>7/2/2025, 8:39:11 PM</v>
+        <v>7/2/2025, 8:39:36 PM</v>
       </c>
       <c r="K74">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>326</v>
+        <v>379</v>
       </c>
       <c r="B75">
         <v>5</v>
@@ -3035,18 +3035,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I75" t="str">
-        <v>JE Dunn Maintenance &amp; Support - Bench from 10th June</v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J75" t="str">
-        <v>7/2/2025, 8:39:36 PM</v>
+        <v>7/3/2025, 1:21:56 PM</v>
       </c>
       <c r="K75">
-        <v>52</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>379</v>
+        <v>344</v>
       </c>
       <c r="B76">
         <v>5</v>
@@ -3070,18 +3070,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I76" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
+        <v>Placemaker Buffer - Will be 100% billable from Mid July</v>
       </c>
       <c r="J76" t="str">
-        <v>7/3/2025, 1:21:56 PM</v>
+        <v>7/3/2025, 1:28:51 PM</v>
       </c>
       <c r="K76">
-        <v>109</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="B77">
         <v>5</v>
@@ -3105,10 +3105,10 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I77" t="str">
-        <v>Placemaker Buffer - Will be 100% billable from Mid July</v>
+        <v xml:space="preserve">Training on SAP S4 Hana -  Back up  Bench - Less cost  </v>
       </c>
       <c r="J77" t="str">
-        <v>7/3/2025, 1:28:51 PM</v>
+        <v>7/3/2025, 1:31:46 PM</v>
       </c>
       <c r="K77">
         <v>55</v>
@@ -3116,16 +3116,16 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C78" t="str">
-        <v>10000271</v>
+        <v>10000301</v>
       </c>
       <c r="D78" t="str">
-        <v>Kishore Chittabathina</v>
+        <v>Kishore  Sunkara</v>
       </c>
       <c r="E78" t="str">
         <v>AI Innovation</v>
@@ -3137,21 +3137,21 @@
         <v>AI Training</v>
       </c>
       <c r="H78" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I78" t="str">
-        <v xml:space="preserve">Training on SAP S4 Hana -  Back up  Bench - Less cost  </v>
+        <v>Kids delivery</v>
       </c>
       <c r="J78" t="str">
-        <v>7/3/2025, 1:31:46 PM</v>
+        <v>6/23/2025, 6:47:45 PM</v>
       </c>
       <c r="K78">
-        <v>55</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="B79">
         <v>7</v>
@@ -3175,18 +3175,18 @@
         <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I79" t="str">
-        <v>Kids delivery</v>
+        <v>from June mapped into August Shopify Plugin</v>
       </c>
       <c r="J79" t="str">
-        <v>6/23/2025, 6:47:45 PM</v>
+        <v>6/23/2025, 6:49:00 PM</v>
       </c>
       <c r="K79">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>342</v>
+        <v>271</v>
       </c>
       <c r="B80">
         <v>7</v>
@@ -3207,21 +3207,21 @@
         <v>AI Training</v>
       </c>
       <c r="H80" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I80" t="str">
-        <v>from June mapped into August Shopify Plugin</v>
+        <v xml:space="preserve">Billable under  JE Dune , Richarson </v>
       </c>
       <c r="J80" t="str">
-        <v>6/23/2025, 6:49:00 PM</v>
+        <v>6/25/2025, 7:51:11 PM</v>
       </c>
       <c r="K80">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>271</v>
+        <v>301</v>
       </c>
       <c r="B81">
         <v>7</v>
@@ -3245,18 +3245,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I81" t="str">
-        <v xml:space="preserve">Billable under  JE Dune , Richarson </v>
+        <v>Managing - Woek Wear, Gallagher, Pet Barn</v>
       </c>
       <c r="J81" t="str">
-        <v>6/25/2025, 7:51:11 PM</v>
+        <v>6/25/2025, 7:52:59 PM</v>
       </c>
       <c r="K81">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>301</v>
+        <v>373</v>
       </c>
       <c r="B82">
         <v>7</v>
@@ -3280,18 +3280,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I82" t="str">
-        <v>Managing - Woek Wear, Gallagher, Pet Barn</v>
+        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
       </c>
       <c r="J82" t="str">
-        <v>6/25/2025, 7:52:59 PM</v>
+        <v>6/25/2025, 8:05:47 PM</v>
       </c>
       <c r="K82">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>373</v>
+        <v>295</v>
       </c>
       <c r="B83">
         <v>7</v>
@@ -3315,18 +3315,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I83" t="str">
-        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
+        <v>Keico (projection) -  (two and half month’s bench)</v>
       </c>
       <c r="J83" t="str">
-        <v>6/25/2025, 8:05:47 PM</v>
+        <v>6/25/2025, 8:07:33 PM</v>
       </c>
       <c r="K83">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="B84">
         <v>7</v>
@@ -3347,21 +3347,21 @@
         <v>AI Training</v>
       </c>
       <c r="H84" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Farhan Ahmed</v>
       </c>
       <c r="I84" t="str">
-        <v>Keico (projection) -  (two and half month’s bench)</v>
+        <v>Test Comment</v>
       </c>
       <c r="J84" t="str">
-        <v>6/25/2025, 8:07:33 PM</v>
+        <v>6/26/2025, 3:36:49 PM</v>
       </c>
       <c r="K84">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="B85">
         <v>7</v>
@@ -3382,21 +3382,21 @@
         <v>AI Training</v>
       </c>
       <c r="H85" t="str">
-        <v>Farhan Ahmed</v>
+        <v>Muhammad Rehman Shahid</v>
       </c>
       <c r="I85" t="str">
-        <v>Test Comment</v>
+        <v>Abdullah is Non Billable.</v>
       </c>
       <c r="J85" t="str">
-        <v>6/26/2025, 3:36:49 PM</v>
+        <v>6/26/2025, 3:54:12 PM</v>
       </c>
       <c r="K85">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>276</v>
+        <v>351</v>
       </c>
       <c r="B86">
         <v>7</v>
@@ -3417,21 +3417,21 @@
         <v>AI Training</v>
       </c>
       <c r="H86" t="str">
-        <v>Muhammad Rehman Shahid</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I86" t="str">
-        <v>Abdullah is Non Billable.</v>
+        <v>Placemaker Buffer - Will be 100% billable from Mid July</v>
       </c>
       <c r="J86" t="str">
-        <v>6/26/2025, 3:54:12 PM</v>
+        <v>7/2/2025, 8:27:34 PM</v>
       </c>
       <c r="K86">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="B87">
         <v>7</v>
@@ -3455,18 +3455,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I87" t="str">
-        <v>Placemaker Buffer - Will be 100% billable from Mid July</v>
+        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
       </c>
       <c r="J87" t="str">
-        <v>7/2/2025, 8:27:34 PM</v>
+        <v>7/2/2025, 8:40:00 PM</v>
       </c>
       <c r="K87">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>335</v>
+        <v>380</v>
       </c>
       <c r="B88">
         <v>7</v>
@@ -3487,21 +3487,21 @@
         <v>AI Training</v>
       </c>
       <c r="H88" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Karthik Venkittu</v>
       </c>
       <c r="I88" t="str">
-        <v>Dimond Roofing + KO Requirements Phase 1.Fletcher Builder - From 16th June on bench</v>
+        <v>Offboarded on 30th June.</v>
       </c>
       <c r="J88" t="str">
-        <v>7/2/2025, 8:40:00 PM</v>
+        <v>7/3/2025, 12:36:39 PM</v>
       </c>
       <c r="K88">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>380</v>
+        <v>314</v>
       </c>
       <c r="B89">
         <v>7</v>
@@ -3525,18 +3525,18 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I89" t="str">
-        <v>Offboarded on 30th June.</v>
+        <v xml:space="preserve">She will be made billable from 1st August in RAC SFB2CComposable Migration project. SOW is in the process. </v>
       </c>
       <c r="J89" t="str">
-        <v>7/3/2025, 12:36:39 PM</v>
+        <v>7/3/2025, 12:56:23 PM</v>
       </c>
       <c r="K89">
-        <v>24</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="B90">
         <v>7</v>
@@ -3557,21 +3557,21 @@
         <v>AI Training</v>
       </c>
       <c r="H90" t="str">
-        <v>Karthik Venkittu</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I90" t="str">
-        <v xml:space="preserve">She will be made billable from 1st August in RAC SFB2CComposable Migration project. SOW is in the process. </v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J90" t="str">
-        <v>7/3/2025, 12:56:23 PM</v>
+        <v>7/3/2025, 1:22:30 PM</v>
       </c>
       <c r="K90">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>368</v>
+        <v>288</v>
       </c>
       <c r="B91">
         <v>7</v>
@@ -3595,27 +3595,27 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I91" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
+        <v>50% Billable in Whilecap . Aslo PM for - Rockwest, UFA</v>
       </c>
       <c r="J91" t="str">
-        <v>7/3/2025, 1:22:30 PM</v>
+        <v>7/3/2025, 1:23:03 PM</v>
       </c>
       <c r="K91">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>288</v>
+        <v>328</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C92" t="str">
-        <v>10000301</v>
+        <v>10000391</v>
       </c>
       <c r="D92" t="str">
-        <v>Kishore  Sunkara</v>
+        <v>Prashanth Janardhanan</v>
       </c>
       <c r="E92" t="str">
         <v>AI Innovation</v>
@@ -3627,21 +3627,21 @@
         <v>AI Training</v>
       </c>
       <c r="H92" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I92" t="str">
-        <v>50% Billable in Whilecap . Aslo PM for - Rockwest, UFA</v>
+        <v>Kids delivery</v>
       </c>
       <c r="J92" t="str">
-        <v>7/3/2025, 1:23:03 PM</v>
+        <v>6/23/2025, 6:47:45 PM</v>
       </c>
       <c r="K92">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="B93">
         <v>8</v>
@@ -3665,18 +3665,18 @@
         <v>Mahaveer Amudhachandran</v>
       </c>
       <c r="I93" t="str">
-        <v>Kids delivery</v>
+        <v>from June mapped into August Shopify Plugin</v>
       </c>
       <c r="J93" t="str">
-        <v>6/23/2025, 6:47:45 PM</v>
+        <v>6/23/2025, 6:49:00 PM</v>
       </c>
       <c r="K93">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>343</v>
+        <v>272</v>
       </c>
       <c r="B94">
         <v>8</v>
@@ -3697,21 +3697,21 @@
         <v>AI Training</v>
       </c>
       <c r="H94" t="str">
-        <v>Mahaveer Amudhachandran</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I94" t="str">
-        <v>from June mapped into August Shopify Plugin</v>
+        <v xml:space="preserve">Billable under  JE Dune , Richarson </v>
       </c>
       <c r="J94" t="str">
-        <v>6/23/2025, 6:49:00 PM</v>
+        <v>6/25/2025, 7:51:11 PM</v>
       </c>
       <c r="K94">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="B95">
         <v>8</v>
@@ -3735,18 +3735,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I95" t="str">
-        <v xml:space="preserve">Billable under  JE Dune , Richarson </v>
+        <v>Managing - Woek Wear, Gallagher, Pet Barn</v>
       </c>
       <c r="J95" t="str">
-        <v>6/25/2025, 7:51:11 PM</v>
+        <v>6/25/2025, 7:52:59 PM</v>
       </c>
       <c r="K95">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>302</v>
+        <v>372</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -3770,18 +3770,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I96" t="str">
-        <v>Managing - Woek Wear, Gallagher, Pet Barn</v>
+        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
       </c>
       <c r="J96" t="str">
-        <v>6/25/2025, 7:52:59 PM</v>
+        <v>6/25/2025, 8:05:46 PM</v>
       </c>
       <c r="K96">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>372</v>
+        <v>294</v>
       </c>
       <c r="B97">
         <v>8</v>
@@ -3805,18 +3805,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I97" t="str">
-        <v xml:space="preserve">Training on SAP S4 Hana - Also back Bench - Less cost  </v>
+        <v>Keico (projection) -  (two and half month’s bench)</v>
       </c>
       <c r="J97" t="str">
-        <v>6/25/2025, 8:05:46 PM</v>
+        <v>6/25/2025, 8:07:32 PM</v>
       </c>
       <c r="K97">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>294</v>
+        <v>357</v>
       </c>
       <c r="B98">
         <v>8</v>
@@ -3840,18 +3840,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I98" t="str">
-        <v>Keico (projection) -  (two and half month’s bench)</v>
+        <v>Shadow resource as per the SOW - Agreed and approved by Finance</v>
       </c>
       <c r="J98" t="str">
-        <v>6/25/2025, 8:07:32 PM</v>
+        <v>6/25/2025, 8:11:13 PM</v>
       </c>
       <c r="K98">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="B99">
         <v>8</v>
@@ -3872,21 +3872,21 @@
         <v>AI Training</v>
       </c>
       <c r="H99" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Farhan Ahmed</v>
       </c>
       <c r="I99" t="str">
-        <v>Shadow resource as per the SOW - Agreed and approved by Finance</v>
+        <v>Test Comment</v>
       </c>
       <c r="J99" t="str">
-        <v>6/25/2025, 8:11:13 PM</v>
+        <v>6/26/2025, 3:36:48 PM</v>
       </c>
       <c r="K99">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="B100">
         <v>8</v>
@@ -3907,21 +3907,21 @@
         <v>AI Training</v>
       </c>
       <c r="H100" t="str">
-        <v>Farhan Ahmed</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I100" t="str">
-        <v>Test Comment</v>
+        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J100" t="str">
-        <v>6/26/2025, 3:36:48 PM</v>
+        <v>7/2/2025, 7:58:21 PM</v>
       </c>
       <c r="K100">
-        <v>12</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>281</v>
+        <v>367</v>
       </c>
       <c r="B101">
         <v>8</v>
@@ -3948,7 +3948,7 @@
         <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
       </c>
       <c r="J101" t="str">
-        <v>7/2/2025, 7:58:21 PM</v>
+        <v>7/2/2025, 7:58:46 PM</v>
       </c>
       <c r="K101">
         <v>109</v>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>367</v>
+        <v>313</v>
       </c>
       <c r="B102">
         <v>8</v>
@@ -3980,18 +3980,18 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I102" t="str">
-        <v>There is no active opportunity at the moment. Mahaveer intends to provide him with AI training - GWA Use case</v>
+        <v>Managing - PlaceMaker &amp; Pet Barn ( AREN) - Cost covered in the Margin</v>
       </c>
       <c r="J102" t="str">
-        <v>7/2/2025, 7:58:46 PM</v>
+        <v>7/2/2025, 8:22:55 PM</v>
       </c>
       <c r="K102">
-        <v>109</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="B103">
         <v>8</v>
@@ -4012,21 +4012,21 @@
         <v>AI Training</v>
       </c>
       <c r="H103" t="str">
-        <v>Kishore Kumar Thirupuraanandan</v>
+        <v>Karthik Venkittu</v>
       </c>
       <c r="I103" t="str">
-        <v>Managing - PlaceMaker &amp; Pet Barn ( AREN) - Cost covered in the Margin</v>
+        <v xml:space="preserve">He handles Proposal Management for entire BU and will be a non billable resource.  </v>
       </c>
       <c r="J103" t="str">
-        <v>7/2/2025, 8:22:55 PM</v>
+        <v>7/3/2025, 12:33:37 PM</v>
       </c>
       <c r="K103">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>336</v>
+        <v>287</v>
       </c>
       <c r="B104">
         <v>8</v>
@@ -4050,27 +4050,27 @@
         <v>Karthik Venkittu</v>
       </c>
       <c r="I104" t="str">
-        <v xml:space="preserve">He handles Proposal Management for entire BU and will be a non billable resource.  </v>
+        <v>Non billable from 23rd June</v>
       </c>
       <c r="J104" t="str">
-        <v>7/3/2025, 12:33:37 PM</v>
+        <v>7/3/2025, 12:57:37 PM</v>
       </c>
       <c r="K104">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>287</v>
+        <v>315</v>
       </c>
       <c r="B105">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C105" t="str">
-        <v>10000391</v>
+        <v>10004311</v>
       </c>
       <c r="D105" t="str">
-        <v>Prashanth Janardhanan</v>
+        <v>Mohammad Bilal G</v>
       </c>
       <c r="E105" t="str">
         <v>AI Innovation</v>
@@ -4082,30 +4082,30 @@
         <v>AI Training</v>
       </c>
       <c r="H105" t="str">
-        <v>Karthik Venkittu</v>
+        <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I105" t="str">
-        <v>Non billable from 23rd June</v>
+        <v xml:space="preserve">There is no active opportunity at the moment. Mahaveer intends to provide him  in Optimizely </v>
       </c>
       <c r="J105" t="str">
-        <v>7/3/2025, 12:57:37 PM</v>
+        <v>6/25/2025, 7:42:31 PM</v>
       </c>
       <c r="K105">
-        <v>27</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>352</v>
+        <v>316</v>
       </c>
       <c r="B106">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="C106" t="str">
-        <v>10008441</v>
+        <v>10004311</v>
       </c>
       <c r="D106" t="str">
-        <v>Praveen M G</v>
+        <v>Mohammad Bilal G</v>
       </c>
       <c r="E106" t="str">
         <v>AI Innovation</v>
@@ -4114,19 +4114,19 @@
         <v>Digital Commerce</v>
       </c>
       <c r="G106" t="str">
-        <v>Petbarn/Shopify</v>
+        <v>AI Training</v>
       </c>
       <c r="H106" t="str">
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I106" t="str">
-        <v>Currently partially billable on the Petbarn project and undergoing training in Shopify</v>
+        <v xml:space="preserve">There is no active opportunity at the moment. Mahaveer intends to provide him  in Optimizely </v>
       </c>
       <c r="J106" t="str">
-        <v>6/25/2025, 7:39:31 PM</v>
+        <v>6/25/2025, 7:42:31 PM</v>
       </c>
       <c r="K106">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107">
@@ -4166,7 +4166,7 @@
     </row>
     <row r="108">
       <c r="A108">
-        <v>315</v>
+        <v>352</v>
       </c>
       <c r="B108">
         <v>80</v>
@@ -4190,13 +4190,13 @@
         <v>Kishore Kumar Thirupuraanandan</v>
       </c>
       <c r="I108" t="str">
-        <v xml:space="preserve">There is no active opportunity at the moment. Mahaveer intends to provide him  in Optimizely </v>
+        <v>Currently partially billable on the Petbarn project and undergoing training in Shopify</v>
       </c>
       <c r="J108" t="str">
-        <v>6/25/2025, 7:42:31 PM</v>
+        <v>6/25/2025, 7:39:31 PM</v>
       </c>
       <c r="K108">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109">
@@ -4306,7 +4306,7 @@
     </row>
     <row r="112">
       <c r="A112">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B112">
         <v>80</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="113">
       <c r="A113">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B113">
         <v>80</v>
@@ -4833,7 +4833,7 @@
         <v>AI Training</v>
       </c>
       <c r="G2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>Yes</v>
@@ -5239,13 +5239,13 @@
         <v>AI Training</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I16" t="str">
-        <v>No Messages</v>
+        <v>6/25/2025</v>
       </c>
     </row>
     <row r="17">
@@ -5326,7 +5326,7 @@
         <v>Petbarn/Shopify</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" t="str">
         <v>Yes</v>
@@ -5498,7 +5498,7 @@
         <v>Employees with Chat Feedback</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -5506,7 +5506,7 @@
         <v>Coverage Percentage</v>
       </c>
       <c r="B5" t="str">
-        <v>40.9%</v>
+        <v>45.5%</v>
       </c>
     </row>
     <row r="6">
@@ -5522,7 +5522,7 @@
         <v>Average Messages per Employee</v>
       </c>
       <c r="B7" t="str">
-        <v>13.7</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="8">
@@ -5550,7 +5550,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5750,13 +5750,13 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B9" t="str">
-        <v>10004311</v>
+        <v>10006691</v>
       </c>
       <c r="C9" t="str">
-        <v>Mohammad Bilal G</v>
+        <v>Khatiza Pathan</v>
       </c>
       <c r="D9" t="str">
         <v>AI Innovation</v>
@@ -5765,7 +5765,7 @@
         <v>Digital Commerce</v>
       </c>
       <c r="F9" t="str">
-        <v>AI Training</v>
+        <v>MENA Bev</v>
       </c>
       <c r="G9" t="str">
         <v>Missing Chat Data</v>
@@ -5773,13 +5773,13 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B10" t="str">
-        <v>10006691</v>
+        <v>10007121</v>
       </c>
       <c r="C10" t="str">
-        <v>Khatiza Pathan</v>
+        <v>Laxman Reddy Seelam</v>
       </c>
       <c r="D10" t="str">
         <v>AI Innovation</v>
@@ -5788,7 +5788,7 @@
         <v>Digital Commerce</v>
       </c>
       <c r="F10" t="str">
-        <v>MENA Bev</v>
+        <v>Arcelik</v>
       </c>
       <c r="G10" t="str">
         <v>Missing Chat Data</v>
@@ -5796,13 +5796,13 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B11" t="str">
-        <v>10007121</v>
+        <v>10010191</v>
       </c>
       <c r="C11" t="str">
-        <v>Laxman Reddy Seelam</v>
+        <v>Abdul Wahab</v>
       </c>
       <c r="D11" t="str">
         <v>AI Innovation</v>
@@ -5811,7 +5811,7 @@
         <v>Digital Commerce</v>
       </c>
       <c r="F11" t="str">
-        <v>Arcelik</v>
+        <v>HD Supply</v>
       </c>
       <c r="G11" t="str">
         <v>Missing Chat Data</v>
@@ -5819,13 +5819,13 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B12" t="str">
-        <v>10010191</v>
+        <v>10010411</v>
       </c>
       <c r="C12" t="str">
-        <v>Abdul Wahab</v>
+        <v>Rukmani Devi Dutta</v>
       </c>
       <c r="D12" t="str">
         <v>AI Innovation</v>
@@ -5834,7 +5834,7 @@
         <v>Digital Commerce</v>
       </c>
       <c r="F12" t="str">
-        <v>HD Supply</v>
+        <v>AI Training</v>
       </c>
       <c r="G12" t="str">
         <v>Missing Chat Data</v>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B13" t="str">
-        <v>10010411</v>
+        <v>10010591</v>
       </c>
       <c r="C13" t="str">
-        <v>Rukmani Devi Dutta</v>
+        <v>Sai Krishna Reddy</v>
       </c>
       <c r="D13" t="str">
         <v>AI Innovation</v>
@@ -5857,38 +5857,15 @@
         <v>Digital Commerce</v>
       </c>
       <c r="F13" t="str">
-        <v>AI Training</v>
+        <v>RAC ACIMA</v>
       </c>
       <c r="G13" t="str">
         <v>Missing Chat Data</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14">
-        <v>101</v>
-      </c>
-      <c r="B14" t="str">
-        <v>10010591</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Sai Krishna Reddy</v>
-      </c>
-      <c r="D14" t="str">
-        <v>AI Innovation</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Digital Commerce</v>
-      </c>
-      <c r="F14" t="str">
-        <v>RAC ACIMA</v>
-      </c>
-      <c r="G14" t="str">
-        <v>Missing Chat Data</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>